<commit_message>
Added new entries in excel
</commit_message>
<xml_diff>
--- a/WithoutSynchronization/src/test/Book1.xlsx
+++ b/WithoutSynchronization/src/test/Book1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danish\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danish\git\test\WithoutSynchronization\src\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Browser</t>
   </si>
@@ -36,6 +36,18 @@
   </si>
   <si>
     <t>https://www.gmail.com</t>
+  </si>
+  <si>
+    <t>TS1</t>
+  </si>
+  <si>
+    <t>Danish</t>
+  </si>
+  <si>
+    <t>TS2</t>
+  </si>
+  <si>
+    <t>Check</t>
   </si>
 </sst>
 </file>
@@ -364,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,6 +403,22 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>

</xml_diff>

<commit_message>
Added 1 more sheet
</commit_message>
<xml_diff>
--- a/WithoutSynchronization/src/test/Book1.xlsx
+++ b/WithoutSynchronization/src/test/Book1.xlsx
@@ -8,9 +8,10 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:I9"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Browser</t>
   </si>
@@ -44,6 +45,18 @@
   </si>
   <si>
     <t>Check</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>Starter</t>
+  </si>
+  <si>
+    <t>TS3</t>
+  </si>
+  <si>
+    <t>Shaharyar</t>
   </si>
 </sst>
 </file>
@@ -375,7 +388,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,11 +428,41 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>